<commit_message>
second commit added browser's exe file, setup the path for config file,setup excel file,added screensh ot capability
</commit_message>
<xml_diff>
--- a/src/main/resources/Resources/TestData/TestData.xlsx
+++ b/src/main/resources/Resources/TestData/TestData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{11AB466C-6CCF-4980-B208-DCAF8A3F6032}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22860" windowHeight="10650"/>
+    <workbookView xWindow="1050" yWindow="1050" windowWidth="20460" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidUserLogin" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>UserName</t>
   </si>
@@ -41,11 +42,14 @@
   <si>
     <t>Pa55w0rd</t>
   </si>
+  <si>
+    <t>runMode</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -356,11 +360,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B7:B8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -373,7 +377,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -393,7 +397,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -430,7 +434,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Excel sheet issue resolved
</commit_message>
<xml_diff>
--- a/src/main/resources/Resources/TestData/TestData.xlsx
+++ b/src/main/resources/Resources/TestData/TestData.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{11AB466C-6CCF-4980-B208-DCAF8A3F6032}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SRS\SRS\src\main\resources\Resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59C993B-A2DE-42C4-858F-55B3652E39F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="1050" windowWidth="20460" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidUserLogin" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,6 @@
     <sheet name="InvalidPasswordLogin" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:W33"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>UserName</t>
   </si>
@@ -44,19 +48,46 @@
   </si>
   <si>
     <t>runMode</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>1011002</t>
+  </si>
+  <si>
+    <t>Log On - Ci Anywhere</t>
+  </si>
+  <si>
+    <t>loginPageTitle</t>
+  </si>
+  <si>
+    <t>homePageTitle</t>
+  </si>
+  <si>
+    <t>Ci Anywhere Workplace</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -79,8 +110,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -361,10 +395,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,49 +467,12 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1011002</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1111002</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>

</xml_diff>